<commit_message>
fix date parsing issue from xlsx
</commit_message>
<xml_diff>
--- a/uploads/Ordres.xlsx
+++ b/uploads/Ordres.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whcsetup\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehdi\Desktop\mahdi\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1671778-24FC-40F3-8449-52712C16685B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2350" windowHeight="220"/>
+    <workbookView xWindow="3276" yWindow="3276" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Nom</t>
   </si>
@@ -53,9 +55,6 @@
     <t>Sté Bourse A1</t>
   </si>
   <si>
-    <t>SICAV</t>
-  </si>
-  <si>
     <t>BANQUE A</t>
   </si>
   <si>
@@ -86,15 +85,9 @@
     <t>08/2008 gestion 3</t>
   </si>
   <si>
-    <t>Catégorie</t>
-  </si>
-  <si>
     <t>Tunisien Libre</t>
   </si>
   <si>
-    <t>Etrnager libre</t>
-  </si>
-  <si>
     <t>Copmte propre</t>
   </si>
   <si>
@@ -110,12 +103,6 @@
     <t>Oui</t>
   </si>
   <si>
-    <t xml:space="preserve"> CMF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IDT </t>
-  </si>
-  <si>
     <t>Teneur_de_compte</t>
   </si>
   <si>
@@ -167,9 +154,6 @@
     <t>hhghg</t>
   </si>
   <si>
-    <t>dddd</t>
-  </si>
-  <si>
     <t>djjjdjd</t>
   </si>
   <si>
@@ -194,16 +178,31 @@
     <t>ssss</t>
   </si>
   <si>
-    <t>hhhh</t>
-  </si>
-  <si>
     <t>u</t>
+  </si>
+  <si>
+    <t>Sté SICAV</t>
+  </si>
+  <si>
+    <t>IDT</t>
+  </si>
+  <si>
+    <t>CMF</t>
+  </si>
+  <si>
+    <t>Categorie</t>
+  </si>
+  <si>
+    <t>OPF</t>
+  </si>
+  <si>
+    <t>Etrange libre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -278,10 +277,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -562,36 +557,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" customWidth="1"/>
-    <col min="2" max="2" width="12.90625" customWidth="1"/>
-    <col min="3" max="3" width="20.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14.81640625" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="20.81640625" customWidth="1"/>
-    <col min="9" max="9" width="17.36328125" customWidth="1"/>
-    <col min="10" max="10" width="18.6328125" customWidth="1"/>
-    <col min="11" max="11" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.77734375" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>33</v>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -606,51 +601,51 @@
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="8">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="2">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I2" s="2">
-        <v>2100614</v>
+        <v>21006145</v>
       </c>
       <c r="J2" s="3">
         <v>43142</v>
@@ -658,40 +653,38 @@
       <c r="K2" s="2">
         <v>20</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="L2" s="2"/>
       <c r="M2" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="8">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I3" s="2">
-        <v>2100614</v>
+        <v>21006145</v>
       </c>
       <c r="J3" s="3">
         <v>43142</v>
@@ -700,36 +693,36 @@
         <v>100</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="8">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>47</v>
+        <v>13</v>
+      </c>
+      <c r="F4" s="2">
+        <v>12</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I4" s="2">
         <v>4408756</v>
@@ -741,36 +734,34 @@
         <v>41666</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="8">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="2">
-        <v>334422</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I5" s="2">
         <v>77777</v>
@@ -782,39 +773,39 @@
         <v>41666</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="8">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
         <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I6" s="2">
-        <v>777777</v>
+        <v>12345678</v>
       </c>
       <c r="J6" s="3">
         <v>43142</v>
@@ -823,36 +814,34 @@
         <v>20</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="8">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I7" s="2">
         <v>77777</v>
@@ -864,36 +853,36 @@
         <v>100</v>
       </c>
       <c r="L7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>27</v>
-      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="8">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="6">
         <v>8</v>
       </c>
       <c r="B8" s="2">
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="I8" s="2">
         <v>7777</v>
@@ -905,36 +894,34 @@
         <v>100</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="8">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
         <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I9" s="2">
         <v>777</v>
@@ -942,29 +929,18 @@
       <c r="J9" s="3">
         <v>43142</v>
       </c>
-      <c r="K9" s="2">
-        <v>41666</v>
-      </c>
+      <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
validate Qte by categorie
</commit_message>
<xml_diff>
--- a/uploads/Ordres.xlsx
+++ b/uploads/Ordres.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehdi\Desktop\mahdi\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1671778-24FC-40F3-8449-52712C16685B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F031FDAD-4E99-4725-BB5D-575D20D56CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3276" yWindow="3276" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>Nom</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Etrange libre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
@@ -561,7 +564,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -737,7 +740,7 @@
         <v>55</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -847,7 +850,7 @@
         <v>77777</v>
       </c>
       <c r="J7" s="3">
-        <v>43142</v>
+        <v>36567</v>
       </c>
       <c r="K7" s="2">
         <v>100</v>

</xml_diff>